<commit_message>
Update Fan BOM Export Excel file
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/导出材料表.xlsx
+++ b/AutoLoader/Contents/Support/导出材料表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18330" windowHeight="6480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18330" windowHeight="6480"/>
   </bookViews>
   <sheets>
     <sheet name="壁式轴流风机" sheetId="2" r:id="rId1"/>
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,21 +102,6 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -199,7 +184,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -210,13 +195,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -227,6 +206,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -512,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -525,7 +507,7 @@
     <col min="5" max="5" width="5.25" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.25" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.25" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23" style="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1" customWidth="1"/>
@@ -533,13 +515,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -557,20 +539,20 @@
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
@@ -586,13 +568,13 @@
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="9"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2"/>
@@ -603,7 +585,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="4"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
@@ -616,7 +598,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="4"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
@@ -629,7 +611,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="4"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
@@ -642,7 +624,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="4"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
@@ -655,7 +637,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
+      <c r="I7" s="4"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
@@ -668,7 +650,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
@@ -681,7 +663,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
@@ -694,7 +676,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="4"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
@@ -707,7 +689,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
+      <c r="I11" s="4"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
@@ -720,7 +702,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="4"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
@@ -733,7 +715,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
@@ -746,7 +728,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="4"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
@@ -759,7 +741,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="4"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
@@ -772,7 +754,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
+      <c r="I16" s="4"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
@@ -785,7 +767,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="4"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
@@ -798,7 +780,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
+      <c r="I18" s="4"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
@@ -811,7 +793,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="3"/>
+      <c r="I19" s="4"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
@@ -824,7 +806,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="3"/>
+      <c r="I20" s="4"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
@@ -837,7 +819,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
+      <c r="I21" s="4"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
@@ -850,7 +832,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="3"/>
+      <c r="I22" s="4"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
@@ -863,7 +845,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="3"/>
+      <c r="I23" s="4"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
@@ -876,7 +858,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="3"/>
+      <c r="I24" s="4"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
@@ -889,7 +871,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="3"/>
+      <c r="I25" s="4"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
@@ -902,7 +884,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="3"/>
+      <c r="I26" s="4"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
@@ -915,7 +897,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="4"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
@@ -928,7 +910,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="3"/>
+      <c r="I28" s="4"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
@@ -941,7 +923,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="3"/>
+      <c r="I29" s="4"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
@@ -954,7 +936,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="3"/>
+      <c r="I30" s="4"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
@@ -967,7 +949,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="3"/>
+      <c r="I31" s="4"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
@@ -980,7 +962,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="3"/>
+      <c r="I32" s="4"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
@@ -993,7 +975,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="3"/>
+      <c r="I33" s="4"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
@@ -1006,7 +988,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="3"/>
+      <c r="I34" s="4"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
@@ -1019,7 +1001,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="3"/>
+      <c r="I35" s="4"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
@@ -1032,7 +1014,7 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="3"/>
+      <c r="I36" s="4"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
@@ -1045,7 +1027,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="3"/>
+      <c r="I37" s="4"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
@@ -1058,7 +1040,7 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="3"/>
+      <c r="I38" s="4"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
@@ -1071,7 +1053,7 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="3"/>
+      <c r="I39" s="4"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
@@ -1084,7 +1066,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="3"/>
+      <c r="I40" s="4"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
@@ -1097,7 +1079,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
-      <c r="I41" s="3"/>
+      <c r="I41" s="4"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
@@ -1110,7 +1092,7 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
-      <c r="I42" s="3"/>
+      <c r="I42" s="4"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
@@ -1123,7 +1105,7 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
-      <c r="I43" s="3"/>
+      <c r="I43" s="4"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
@@ -1136,7 +1118,7 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
-      <c r="I44" s="3"/>
+      <c r="I44" s="4"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
@@ -1149,7 +1131,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="3"/>
+      <c r="I45" s="4"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
@@ -1162,7 +1144,7 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
-      <c r="I46" s="3"/>
+      <c r="I46" s="4"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
@@ -1175,7 +1157,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
-      <c r="I47" s="3"/>
+      <c r="I47" s="4"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
@@ -1188,7 +1170,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
-      <c r="I48" s="3"/>
+      <c r="I48" s="4"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
@@ -1201,7 +1183,7 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
-      <c r="I49" s="3"/>
+      <c r="I49" s="4"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
@@ -1214,7 +1196,7 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
-      <c r="I50" s="3"/>
+      <c r="I50" s="4"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
@@ -1227,7 +1209,7 @@
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
-      <c r="I51" s="3"/>
+      <c r="I51" s="4"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
@@ -1240,7 +1222,7 @@
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
-      <c r="I52" s="3"/>
+      <c r="I52" s="4"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
     </row>
@@ -1253,7 +1235,7 @@
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
-      <c r="I53" s="3"/>
+      <c r="I53" s="4"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
@@ -1266,7 +1248,7 @@
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
-      <c r="I54" s="3"/>
+      <c r="I54" s="4"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
@@ -1279,7 +1261,7 @@
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
-      <c r="I55" s="3"/>
+      <c r="I55" s="4"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
@@ -1292,7 +1274,7 @@
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
-      <c r="I56" s="3"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
@@ -1305,7 +1287,7 @@
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
-      <c r="I57" s="3"/>
+      <c r="I57" s="4"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
@@ -1318,7 +1300,7 @@
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
-      <c r="I58" s="3"/>
+      <c r="I58" s="4"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
@@ -1331,7 +1313,7 @@
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
-      <c r="I59" s="3"/>
+      <c r="I59" s="4"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
     </row>
@@ -1344,7 +1326,7 @@
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
-      <c r="I60" s="3"/>
+      <c r="I60" s="4"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
@@ -1357,7 +1339,7 @@
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
-      <c r="I61" s="3"/>
+      <c r="I61" s="4"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
@@ -1370,7 +1352,7 @@
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
-      <c r="I62" s="3"/>
+      <c r="I62" s="4"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
@@ -1383,7 +1365,7 @@
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
-      <c r="I63" s="3"/>
+      <c r="I63" s="4"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
@@ -1396,7 +1378,7 @@
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
-      <c r="I64" s="3"/>
+      <c r="I64" s="4"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
     </row>
@@ -1409,7 +1391,7 @@
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
-      <c r="I65" s="3"/>
+      <c r="I65" s="4"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
     </row>
@@ -1422,7 +1404,7 @@
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
-      <c r="I66" s="3"/>
+      <c r="I66" s="4"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
     </row>
@@ -1435,7 +1417,7 @@
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
-      <c r="I67" s="3"/>
+      <c r="I67" s="4"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
     </row>
@@ -1448,7 +1430,7 @@
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
-      <c r="I68" s="3"/>
+      <c r="I68" s="4"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
@@ -1461,7 +1443,7 @@
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
-      <c r="I69" s="3"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
@@ -1474,7 +1456,7 @@
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
-      <c r="I70" s="3"/>
+      <c r="I70" s="4"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
@@ -1487,7 +1469,7 @@
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
-      <c r="I71" s="3"/>
+      <c r="I71" s="4"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
@@ -1500,7 +1482,7 @@
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
-      <c r="I72" s="3"/>
+      <c r="I72" s="4"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
@@ -1513,7 +1495,7 @@
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
-      <c r="I73" s="3"/>
+      <c r="I73" s="4"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
@@ -1526,7 +1508,7 @@
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
-      <c r="I74" s="3"/>
+      <c r="I74" s="4"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
@@ -1539,7 +1521,7 @@
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
-      <c r="I75" s="3"/>
+      <c r="I75" s="4"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
     </row>
@@ -1552,7 +1534,7 @@
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
-      <c r="I76" s="3"/>
+      <c r="I76" s="4"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
     </row>
@@ -1565,7 +1547,7 @@
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
-      <c r="I77" s="3"/>
+      <c r="I77" s="4"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
@@ -1578,7 +1560,7 @@
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
-      <c r="I78" s="3"/>
+      <c r="I78" s="4"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
@@ -1591,7 +1573,7 @@
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
-      <c r="I79" s="3"/>
+      <c r="I79" s="4"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
@@ -1604,7 +1586,7 @@
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
-      <c r="I80" s="3"/>
+      <c r="I80" s="4"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
     </row>
@@ -1617,7 +1599,7 @@
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
-      <c r="I81" s="3"/>
+      <c r="I81" s="4"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
     </row>
@@ -1630,7 +1612,7 @@
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
-      <c r="I82" s="3"/>
+      <c r="I82" s="4"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
@@ -1643,7 +1625,7 @@
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
-      <c r="I83" s="3"/>
+      <c r="I83" s="4"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
@@ -1656,7 +1638,7 @@
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
-      <c r="I84" s="3"/>
+      <c r="I84" s="4"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
@@ -1669,7 +1651,7 @@
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
-      <c r="I85" s="3"/>
+      <c r="I85" s="4"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
@@ -1682,7 +1664,7 @@
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
-      <c r="I86" s="3"/>
+      <c r="I86" s="4"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
@@ -1695,7 +1677,7 @@
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
-      <c r="I87" s="3"/>
+      <c r="I87" s="4"/>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
@@ -1708,7 +1690,7 @@
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
-      <c r="I88" s="3"/>
+      <c r="I88" s="4"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
@@ -1721,7 +1703,7 @@
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
-      <c r="I89" s="3"/>
+      <c r="I89" s="4"/>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
@@ -1734,7 +1716,7 @@
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
-      <c r="I90" s="3"/>
+      <c r="I90" s="4"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
@@ -1747,7 +1729,7 @@
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
-      <c r="I91" s="3"/>
+      <c r="I91" s="4"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
@@ -1760,7 +1742,7 @@
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
-      <c r="I92" s="3"/>
+      <c r="I92" s="4"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
@@ -1773,7 +1755,7 @@
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
-      <c r="I93" s="3"/>
+      <c r="I93" s="4"/>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
@@ -1786,7 +1768,7 @@
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
-      <c r="I94" s="3"/>
+      <c r="I94" s="4"/>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
@@ -1799,7 +1781,7 @@
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
-      <c r="I95" s="3"/>
+      <c r="I95" s="4"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
@@ -1812,7 +1794,7 @@
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
-      <c r="I96" s="3"/>
+      <c r="I96" s="4"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
     </row>
@@ -1825,7 +1807,7 @@
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
-      <c r="I97" s="3"/>
+      <c r="I97" s="4"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
@@ -1838,7 +1820,7 @@
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
-      <c r="I98" s="3"/>
+      <c r="I98" s="4"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
@@ -1859,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1872,21 +1854,20 @@
     <col min="5" max="5" width="5.25" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.25" style="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1904,20 +1885,20 @@
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1933,13 +1914,13 @@
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="9"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2"/>
@@ -1950,8 +1931,8 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="2"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11">
@@ -1963,8 +1944,8 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="2"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11">
@@ -1976,8 +1957,8 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="2"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
@@ -1989,8 +1970,8 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="2"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11">
@@ -2002,8 +1983,8 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="2"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11">
@@ -2015,8 +1996,8 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="2"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11">
@@ -2028,8 +2009,8 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="2"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="3"/>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11">
@@ -2041,8 +2022,8 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="2"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11">
@@ -2054,8 +2035,8 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="2"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11">
@@ -2067,8 +2048,8 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="2"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="3"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11">
@@ -2080,8 +2061,8 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="2"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="3"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11">
@@ -2093,8 +2074,8 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="2"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11">
@@ -2106,8 +2087,8 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="2"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="3"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11">
@@ -2119,8 +2100,8 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="2"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="3"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11">
@@ -2132,8 +2113,8 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="2"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="3"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11">
@@ -2145,8 +2126,8 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="2"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="3"/>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11">
@@ -2158,8 +2139,8 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="2"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="3"/>
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
@@ -2171,8 +2152,8 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="2"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="3"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
@@ -2184,8 +2165,8 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="2"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="3"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11">
@@ -2197,8 +2178,8 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="2"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="3"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11">
@@ -2210,8 +2191,8 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="2"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="3"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11">
@@ -2223,8 +2204,8 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="2"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="3"/>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11">
@@ -2236,8 +2217,8 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="2"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="3"/>
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11">
@@ -2249,8 +2230,8 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="2"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="3"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11">
@@ -2262,8 +2243,8 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="2"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="3"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11">
@@ -2275,8 +2256,8 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="2"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="3"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11">
@@ -2288,8 +2269,8 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="2"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="3"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11">
@@ -2301,8 +2282,8 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="2"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="3"/>
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11">
@@ -2314,8 +2295,8 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="2"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="3"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11">
@@ -2327,8 +2308,8 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="2"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="3"/>
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:11">
@@ -2340,8 +2321,8 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="2"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="3"/>
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:11">
@@ -2353,8 +2334,8 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="2"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="3"/>
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11">
@@ -2366,8 +2347,8 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="2"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="3"/>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11">
@@ -2379,8 +2360,8 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="2"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="3"/>
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11">
@@ -2392,8 +2373,8 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="2"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="3"/>
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:11">
@@ -2405,8 +2386,8 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="2"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="3"/>
       <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:11">
@@ -2418,8 +2399,8 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="2"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="3"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11">
@@ -2431,8 +2412,8 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="2"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="3"/>
       <c r="K40" s="2"/>
     </row>
     <row r="41" spans="1:11">
@@ -2444,8 +2425,8 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="2"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="3"/>
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11">
@@ -2457,8 +2438,8 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="2"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="3"/>
       <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11">
@@ -2470,8 +2451,8 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="2"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="3"/>
       <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11">
@@ -2483,8 +2464,8 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="2"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="3"/>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11">
@@ -2496,8 +2477,8 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="2"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="3"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11">
@@ -2509,8 +2490,8 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="2"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="3"/>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:11">
@@ -2522,8 +2503,8 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="2"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="3"/>
       <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:11">
@@ -2535,8 +2516,8 @@
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="2"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="3"/>
       <c r="K48" s="2"/>
     </row>
     <row r="49" spans="1:11">
@@ -2548,8 +2529,8 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="2"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="3"/>
       <c r="K49" s="2"/>
     </row>
     <row r="50" spans="1:11">
@@ -2561,8 +2542,8 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="2"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="3"/>
       <c r="K50" s="2"/>
     </row>
     <row r="51" spans="1:11">
@@ -2574,8 +2555,8 @@
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="2"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="3"/>
       <c r="K51" s="2"/>
     </row>
     <row r="52" spans="1:11">
@@ -2587,8 +2568,8 @@
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="2"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="3"/>
       <c r="K52" s="2"/>
     </row>
     <row r="53" spans="1:11">
@@ -2600,8 +2581,8 @@
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="2"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="3"/>
       <c r="K53" s="2"/>
     </row>
     <row r="54" spans="1:11">
@@ -2613,8 +2594,8 @@
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="2"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="3"/>
       <c r="K54" s="2"/>
     </row>
     <row r="55" spans="1:11">
@@ -2626,8 +2607,8 @@
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="2"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="3"/>
       <c r="K55" s="2"/>
     </row>
     <row r="56" spans="1:11">
@@ -2639,8 +2620,8 @@
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="2"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="3"/>
       <c r="K56" s="2"/>
     </row>
     <row r="57" spans="1:11">
@@ -2652,8 +2633,8 @@
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="2"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="3"/>
       <c r="K57" s="2"/>
     </row>
     <row r="58" spans="1:11">
@@ -2665,8 +2646,8 @@
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="2"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="3"/>
       <c r="K58" s="2"/>
     </row>
     <row r="59" spans="1:11">
@@ -2678,8 +2659,8 @@
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="2"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="3"/>
       <c r="K59" s="2"/>
     </row>
     <row r="60" spans="1:11">
@@ -2691,8 +2672,8 @@
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="2"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="3"/>
       <c r="K60" s="2"/>
     </row>
     <row r="61" spans="1:11">
@@ -2704,8 +2685,8 @@
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="2"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="3"/>
       <c r="K61" s="2"/>
     </row>
     <row r="62" spans="1:11">
@@ -2717,8 +2698,8 @@
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="2"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="3"/>
       <c r="K62" s="2"/>
     </row>
     <row r="63" spans="1:11">
@@ -2730,8 +2711,8 @@
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="2"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="3"/>
       <c r="K63" s="2"/>
     </row>
     <row r="64" spans="1:11">
@@ -2743,8 +2724,8 @@
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="2"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="3"/>
       <c r="K64" s="2"/>
     </row>
     <row r="65" spans="1:11">
@@ -2756,8 +2737,8 @@
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="2"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="3"/>
       <c r="K65" s="2"/>
     </row>
     <row r="66" spans="1:11">
@@ -2769,8 +2750,8 @@
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="2"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="3"/>
       <c r="K66" s="2"/>
     </row>
     <row r="67" spans="1:11">
@@ -2782,8 +2763,8 @@
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="2"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="3"/>
       <c r="K67" s="2"/>
     </row>
     <row r="68" spans="1:11">
@@ -2795,8 +2776,8 @@
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="2"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="3"/>
       <c r="K68" s="2"/>
     </row>
     <row r="69" spans="1:11">
@@ -2808,8 +2789,8 @@
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="2"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="3"/>
       <c r="K69" s="2"/>
     </row>
     <row r="70" spans="1:11">
@@ -2821,8 +2802,8 @@
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
-      <c r="I70" s="3"/>
-      <c r="J70" s="2"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="3"/>
       <c r="K70" s="2"/>
     </row>
     <row r="71" spans="1:11">
@@ -2834,8 +2815,8 @@
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="2"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="3"/>
       <c r="K71" s="2"/>
     </row>
     <row r="72" spans="1:11">
@@ -2847,8 +2828,8 @@
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="2"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="3"/>
       <c r="K72" s="2"/>
     </row>
     <row r="73" spans="1:11">
@@ -2860,8 +2841,8 @@
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="2"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="3"/>
       <c r="K73" s="2"/>
     </row>
     <row r="74" spans="1:11">
@@ -2873,8 +2854,8 @@
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="2"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="3"/>
       <c r="K74" s="2"/>
     </row>
     <row r="75" spans="1:11">
@@ -2886,8 +2867,8 @@
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
-      <c r="I75" s="3"/>
-      <c r="J75" s="2"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="3"/>
       <c r="K75" s="2"/>
     </row>
     <row r="76" spans="1:11">
@@ -2899,8 +2880,8 @@
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
-      <c r="I76" s="3"/>
-      <c r="J76" s="2"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="3"/>
       <c r="K76" s="2"/>
     </row>
     <row r="77" spans="1:11">
@@ -2912,8 +2893,8 @@
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
-      <c r="I77" s="3"/>
-      <c r="J77" s="2"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="3"/>
       <c r="K77" s="2"/>
     </row>
     <row r="78" spans="1:11">
@@ -2925,8 +2906,8 @@
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="2"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="3"/>
       <c r="K78" s="2"/>
     </row>
     <row r="79" spans="1:11">
@@ -2938,8 +2919,8 @@
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
-      <c r="I79" s="3"/>
-      <c r="J79" s="2"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="3"/>
       <c r="K79" s="2"/>
     </row>
     <row r="80" spans="1:11">
@@ -2951,8 +2932,8 @@
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="2"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="3"/>
       <c r="K80" s="2"/>
     </row>
     <row r="81" spans="1:11">
@@ -2964,8 +2945,8 @@
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
-      <c r="I81" s="3"/>
-      <c r="J81" s="2"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="3"/>
       <c r="K81" s="2"/>
     </row>
     <row r="82" spans="1:11">
@@ -2977,8 +2958,8 @@
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="2"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="3"/>
       <c r="K82" s="2"/>
     </row>
     <row r="83" spans="1:11">
@@ -2990,8 +2971,8 @@
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
-      <c r="I83" s="3"/>
-      <c r="J83" s="2"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="3"/>
       <c r="K83" s="2"/>
     </row>
     <row r="84" spans="1:11">
@@ -3003,8 +2984,8 @@
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
-      <c r="I84" s="3"/>
-      <c r="J84" s="2"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="3"/>
       <c r="K84" s="2"/>
     </row>
     <row r="85" spans="1:11">
@@ -3016,8 +2997,8 @@
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
-      <c r="I85" s="3"/>
-      <c r="J85" s="2"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="3"/>
       <c r="K85" s="2"/>
     </row>
     <row r="86" spans="1:11">
@@ -3029,8 +3010,8 @@
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
-      <c r="I86" s="3"/>
-      <c r="J86" s="2"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="3"/>
       <c r="K86" s="2"/>
     </row>
     <row r="87" spans="1:11">
@@ -3042,8 +3023,8 @@
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
-      <c r="I87" s="3"/>
-      <c r="J87" s="2"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="3"/>
       <c r="K87" s="2"/>
     </row>
     <row r="88" spans="1:11">
@@ -3055,8 +3036,8 @@
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
-      <c r="I88" s="3"/>
-      <c r="J88" s="2"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="3"/>
       <c r="K88" s="2"/>
     </row>
     <row r="89" spans="1:11">
@@ -3068,8 +3049,8 @@
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
-      <c r="I89" s="3"/>
-      <c r="J89" s="2"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="3"/>
       <c r="K89" s="2"/>
     </row>
     <row r="90" spans="1:11">
@@ -3081,8 +3062,8 @@
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="2"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="3"/>
       <c r="K90" s="2"/>
     </row>
     <row r="91" spans="1:11">
@@ -3094,8 +3075,8 @@
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
-      <c r="I91" s="3"/>
-      <c r="J91" s="2"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="3"/>
       <c r="K91" s="2"/>
     </row>
     <row r="92" spans="1:11">
@@ -3107,8 +3088,8 @@
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
-      <c r="I92" s="3"/>
-      <c r="J92" s="2"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="3"/>
       <c r="K92" s="2"/>
     </row>
     <row r="93" spans="1:11">
@@ -3120,8 +3101,8 @@
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
-      <c r="I93" s="3"/>
-      <c r="J93" s="2"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="3"/>
       <c r="K93" s="2"/>
     </row>
     <row r="94" spans="1:11">
@@ -3133,8 +3114,8 @@
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
-      <c r="I94" s="3"/>
-      <c r="J94" s="2"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="3"/>
       <c r="K94" s="2"/>
     </row>
     <row r="95" spans="1:11">
@@ -3146,8 +3127,8 @@
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
-      <c r="I95" s="3"/>
-      <c r="J95" s="2"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="3"/>
       <c r="K95" s="2"/>
     </row>
     <row r="96" spans="1:11">
@@ -3159,8 +3140,8 @@
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
-      <c r="I96" s="3"/>
-      <c r="J96" s="2"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="3"/>
       <c r="K96" s="2"/>
     </row>
     <row r="97" spans="1:11">
@@ -3172,8 +3153,8 @@
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
-      <c r="I97" s="3"/>
-      <c r="J97" s="2"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="3"/>
       <c r="K97" s="2"/>
     </row>
     <row r="98" spans="1:11">
@@ -3185,8 +3166,8 @@
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
-      <c r="I98" s="3"/>
-      <c r="J98" s="2"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="3"/>
       <c r="K98" s="2"/>
     </row>
   </sheetData>
@@ -3198,7 +3179,7 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3207,7 +3188,7 @@
   <dimension ref="A1:J98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3218,20 +3199,21 @@
     <col min="4" max="4" width="5.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.25" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.875" style="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -3246,20 +3228,20 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3272,13 +3254,13 @@
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="9"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2"/>
@@ -3288,7 +3270,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
@@ -3300,7 +3282,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
@@ -3312,7 +3294,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
@@ -3324,7 +3306,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
@@ -3336,7 +3318,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
@@ -3348,7 +3330,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="3"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
@@ -3360,7 +3342,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
@@ -3372,7 +3354,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="H10" s="3"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
@@ -3384,7 +3366,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="H11" s="3"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
@@ -3396,7 +3378,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="3"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
@@ -3408,7 +3390,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
@@ -3420,7 +3402,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="H14" s="3"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
@@ -3432,7 +3414,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
@@ -3444,7 +3426,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="3"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
@@ -3456,7 +3438,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
@@ -3468,7 +3450,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="H18" s="3"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
@@ -3480,7 +3462,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="H19" s="3"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
@@ -3492,7 +3474,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="H20" s="3"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
@@ -3504,7 +3486,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
@@ -3516,7 +3498,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="H22" s="3"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
@@ -3528,7 +3510,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="H23" s="3"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
@@ -3540,7 +3522,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="H24" s="3"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
@@ -3552,7 +3534,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="H25" s="3"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
@@ -3564,7 +3546,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="H26" s="3"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
@@ -3576,7 +3558,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="H27" s="3"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
@@ -3588,7 +3570,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="H28" s="3"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
@@ -3600,7 +3582,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="H29" s="3"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
@@ -3612,7 +3594,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="H30" s="3"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
@@ -3624,7 +3606,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="H31" s="3"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
@@ -3636,7 +3618,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="H32" s="3"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
@@ -3648,7 +3630,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
+      <c r="H33" s="3"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
@@ -3660,7 +3642,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="H34" s="3"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
@@ -3672,7 +3654,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+      <c r="H35" s="3"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
@@ -3684,7 +3666,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
+      <c r="H36" s="3"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
@@ -3696,7 +3678,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
+      <c r="H37" s="3"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
@@ -3708,7 +3690,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="H38" s="3"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
@@ -3720,7 +3702,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
+      <c r="H39" s="3"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
@@ -3732,7 +3714,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
+      <c r="H40" s="3"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
@@ -3744,7 +3726,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
+      <c r="H41" s="3"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
@@ -3756,7 +3738,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
+      <c r="H42" s="3"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
@@ -3768,7 +3750,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
+      <c r="H43" s="3"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
@@ -3780,7 +3762,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
+      <c r="H44" s="3"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
@@ -3792,7 +3774,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
+      <c r="H45" s="3"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
@@ -3804,7 +3786,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
+      <c r="H46" s="3"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
@@ -3816,7 +3798,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
+      <c r="H47" s="3"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
@@ -3828,7 +3810,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
+      <c r="H48" s="3"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
@@ -3840,7 +3822,7 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
+      <c r="H49" s="3"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
@@ -3852,7 +3834,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
+      <c r="H50" s="3"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
@@ -3864,7 +3846,7 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
+      <c r="H51" s="3"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
@@ -3876,7 +3858,7 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
+      <c r="H52" s="3"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
@@ -3888,7 +3870,7 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
+      <c r="H53" s="3"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
@@ -3900,7 +3882,7 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
+      <c r="H54" s="3"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
@@ -3912,7 +3894,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
+      <c r="H55" s="3"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
     </row>
@@ -3924,7 +3906,7 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
+      <c r="H56" s="3"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
@@ -3936,7 +3918,7 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
+      <c r="H57" s="3"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
     </row>
@@ -3948,7 +3930,7 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
+      <c r="H58" s="3"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
@@ -3960,7 +3942,7 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
+      <c r="H59" s="3"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
@@ -3972,7 +3954,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
+      <c r="H60" s="3"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
     </row>
@@ -3984,7 +3966,7 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
+      <c r="H61" s="3"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
     </row>
@@ -3996,7 +3978,7 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
+      <c r="H62" s="3"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
@@ -4008,7 +3990,7 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
+      <c r="H63" s="3"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
@@ -4020,7 +4002,7 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
+      <c r="H64" s="3"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
@@ -4032,7 +4014,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
+      <c r="H65" s="3"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
@@ -4044,7 +4026,7 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
+      <c r="H66" s="3"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
     </row>
@@ -4056,7 +4038,7 @@
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
+      <c r="H67" s="3"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
     </row>
@@ -4068,7 +4050,7 @@
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
+      <c r="H68" s="3"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
     </row>
@@ -4080,7 +4062,7 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
+      <c r="H69" s="3"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
     </row>
@@ -4092,7 +4074,7 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
+      <c r="H70" s="3"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
     </row>
@@ -4104,7 +4086,7 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
+      <c r="H71" s="3"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
@@ -4116,7 +4098,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
+      <c r="H72" s="3"/>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
     </row>
@@ -4128,7 +4110,7 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
+      <c r="H73" s="3"/>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
     </row>
@@ -4140,7 +4122,7 @@
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
+      <c r="H74" s="3"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
     </row>
@@ -4152,7 +4134,7 @@
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
+      <c r="H75" s="3"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
     </row>
@@ -4164,7 +4146,7 @@
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
+      <c r="H76" s="3"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
     </row>
@@ -4176,7 +4158,7 @@
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
+      <c r="H77" s="3"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
     </row>
@@ -4188,7 +4170,7 @@
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
+      <c r="H78" s="3"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
     </row>
@@ -4200,7 +4182,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
+      <c r="H79" s="3"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
     </row>
@@ -4212,7 +4194,7 @@
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
+      <c r="H80" s="3"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
     </row>
@@ -4224,7 +4206,7 @@
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
+      <c r="H81" s="3"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
     </row>
@@ -4236,7 +4218,7 @@
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
+      <c r="H82" s="3"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
     </row>
@@ -4248,7 +4230,7 @@
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
+      <c r="H83" s="3"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
     </row>
@@ -4260,7 +4242,7 @@
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
+      <c r="H84" s="3"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
     </row>
@@ -4272,7 +4254,7 @@
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
+      <c r="H85" s="3"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
     </row>
@@ -4284,7 +4266,7 @@
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
+      <c r="H86" s="3"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
     </row>
@@ -4296,7 +4278,7 @@
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
+      <c r="H87" s="3"/>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
     </row>
@@ -4308,7 +4290,7 @@
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
+      <c r="H88" s="3"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
     </row>
@@ -4320,7 +4302,7 @@
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
+      <c r="H89" s="3"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
     </row>
@@ -4332,7 +4314,7 @@
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
+      <c r="H90" s="3"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
     </row>
@@ -4344,7 +4326,7 @@
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
+      <c r="H91" s="3"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
     </row>
@@ -4356,7 +4338,7 @@
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
+      <c r="H92" s="3"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
     </row>
@@ -4368,7 +4350,7 @@
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
+      <c r="H93" s="3"/>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
     </row>
@@ -4380,7 +4362,7 @@
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
+      <c r="H94" s="3"/>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
     </row>
@@ -4392,7 +4374,7 @@
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
+      <c r="H95" s="3"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
     </row>
@@ -4404,7 +4386,7 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
+      <c r="H96" s="3"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
     </row>
@@ -4416,7 +4398,7 @@
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
+      <c r="H97" s="3"/>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
     </row>
@@ -4428,7 +4410,7 @@
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
+      <c r="H98" s="3"/>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
     </row>

</xml_diff>